<commit_message>
Update des question, ajout endocrino et digestif
</commit_message>
<xml_diff>
--- a/Physiopathologie/Excel/cardiaque.xlsx
+++ b/Physiopathologie/Excel/cardiaque.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moito\Desktop\Sérieux\Projet\Site web\Physiopathologie\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE3147D-C984-4DE4-8392-EC4C6C9DD3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B5D2BA-0D5A-48D3-872A-24CA7D7CB91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C1EC4D3-5916-499C-9244-5ABC4AEA4E79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="403">
   <si>
     <t>Numero</t>
   </si>
@@ -734,27 +734,15 @@
     <t xml:space="preserve"> Le système orthosympathique innerve les cardiomyocytes auriculaires et ventriculaires, le nœud sinusal et le  nœud auriculo-ventriculaire, par effet Beta-2.   </t>
   </si>
   <si>
-    <t xml:space="preserve"> La circulation pulmonaire est une circulation à haut débit et à basse pression.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Q34. Concernant l'hémodynamique: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Selon la relation de Laplace appliquée au ventricule, &amp; est la contrainte qui s'exerce au niveau de la paroi et qui est proportionnelle à l'épaisseur de cette paroi.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Selon la relation de Poiseuille-Hagen, lorsque le rayon d'un vaisseau est doublé, le débit sanguin est multiplié  par 16.   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> La vitesse du courant sanguin est de l'ordre de 0,5 mm/sec au niveau du réseau capillaire.    </t>
   </si>
   <si>
     <t xml:space="preserve">Q31. Concernant l'activité électrique cardiaque:  </t>
   </si>
   <si>
-    <t xml:space="preserve"> Lorsque le complexe QRS est positif en DI et est positif en a VF, l'axe du cœur se situe entre O et -30°    </t>
-  </si>
-  <si>
     <t xml:space="preserve"> En absence d'onde P visible à l'ECG, le rythme peut être sinusal.    </t>
   </si>
   <si>
@@ -770,9 +758,6 @@
     <t xml:space="preserve"> Les artérioles représentent le lieu principal de la résistance à l'écoulement du sang dans la mesure où la chute  de pression qui s'exerce à leur niveau est la plus importante,   </t>
   </si>
   <si>
-    <t xml:space="preserve"> Le débit sanguin de circulation pulmonaire est toujours égal au débit sanguin de la circulation systémique dans la mesure où ces deux circulations sont en série.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Q26. Concernant la pompe cardiaque:  </t>
   </si>
   <si>
@@ -797,24 +782,12 @@
     <t xml:space="preserve"> Dans les conditions physiologiques, les sarcomères du cardiomyocyte ont une longueur de 0,9 um, ce qui permet d'augmenter leur tension active lorsque la fibre est étirée jusqu'à 2.2-2,4 um.    </t>
   </si>
   <si>
-    <t xml:space="preserve"> Le premier bruit du cœur est lié à la fermeture des valves aortique et pulmonaire.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La durée d’un cycle cardiaque est l'inverse de la fréquence cardiaque.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Le volume télésystolique normal et au repos est de l'ordre de 50 à 60 ml.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Q4,. En considérant le ventricule, caractériser par Vrai ou Faux chacune des propositions suivantes.  </t>
   </si>
   <si>
     <t xml:space="preserve"> Une augmentation de l’élastance diminue le volume télédiastolique pour une pression télédiastolique donnée.   </t>
   </si>
   <si>
-    <t xml:space="preserve"> Une hypertension artérielle au long cours conduit à une hypertrophie du ventricule gauche qui débouche sur une diminution de la postcharge et de la précharge.   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Modifier la droite d'élastance de fin de systole revient à changer la contractilité.    </t>
   </si>
   <si>
@@ -836,9 +809,6 @@
     <t xml:space="preserve"> Si le débit cardiaque est de 10 L/minute, la fréquence cardiaque de 100/minute et le volume télédiastolique de 150 mil, alors la fraction d'éjection est de 66%.   </t>
   </si>
   <si>
-    <t xml:space="preserve"> Une fraction d'éjection de 30% peut se voir dans une sténose aortique du fait d’une contrainte o du ventricule  gauche augmentée même si la tension artérielle est basse.   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> La fraction d'éjection est souvent conservée dans la dysfonction diastolique alors que le débit cardiaque est diminué.    </t>
   </si>
   <si>
@@ -893,9 +863,6 @@
     <t xml:space="preserve">Q36. En considérant la régulation parasympathique et sympathique du cœur, caractériser par Vrai ou Faux chacune des propositions suivantes.  </t>
   </si>
   <si>
-    <t xml:space="preserve"> Le tonus orthosympathique détermine la fréquence cardiaque de repos.   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Inotrope ou contractilité, chronotrope ou vitesse de conduction et dromotrope ou fréquence cardiaque: ces trois caractéristiques sont activées par la stimulation orthosympathique.   </t>
   </si>
   <si>
@@ -911,33 +878,6 @@
     <t xml:space="preserve"> Un médicament inotrope positif qui augmente le volume d'éjection systolique est excellent pour la perfusion coronaire.   </t>
   </si>
   <si>
-    <t xml:space="preserve"> L'essentiel de l'énergie dépensée par le cœur se produit pendant la phase d'éjection ventriculaire.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q30. En considérant le muscle cardiaque, la précharge, la postcharge et la contractilité, caractériser par  ou  chacune des propositions suivantes.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Par comparaison avec l'augmentation du raccourcissement d'une fibre myocardique isolée sous l'effet d'un agent inotrope, on utilisera l'amélioration de la fraction d'éjection à l'échelon du ventricule entier.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> L'augmentation isolée de la précharge implique une augmentation du volume d'éjection systolique à une vitesse  d'éjection plus rapide jusqu'à un volume télésystolique plus petit.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> L'augmentation isolée de la postcharge implique un volume télésystolique plus grand et une vitesse d’éjection moins rapide.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q28. En considérant le ventricule, caractériser par Vrai ou Faux chacune des propositions suivantes.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La postcharge correspond au © du ventricule gauche durant tout le temps de l’éjection ventriculaire.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La dilatation du ventricule augmente la postcharge et la précharge.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Précharge, postcharge et contractilité sont liées. Par exemple, une augmentation de la postcharge mène immédiatement à une augmentation de la précharge qui est suffisante pour corriger le volume d'éjection systolique.    </t>
-  </si>
-  <si>
     <t>La pression artériel pulsée est proportionnelle au VES et à la compliance aortique</t>
   </si>
   <si>
@@ -1260,6 +1200,51 @@
   </si>
   <si>
     <t xml:space="preserve"> Au niveau de la fibre musculaire cardiaque, la noradrénaline augmente Vmax mais sans modifier la tension isométrique maximale,    </t>
+  </si>
+  <si>
+    <t>"de l'ordre" donc 0,03cm/s est equivalent à 0,5mm/sec</t>
+  </si>
+  <si>
+    <t>L'importance du raccourcissement de la fibre devient le volume ejecté systolique</t>
+  </si>
+  <si>
+    <t>Indépendant, (inotropisme = contractilité)</t>
+  </si>
+  <si>
+    <t>systolique tres haut mais diastolique tres bas</t>
+  </si>
+  <si>
+    <t>askip c vrai</t>
+  </si>
+  <si>
+    <t>Les vasodilatateurs diminuent la résistance périphérique totale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Une fraction d'éjection de 30% peut se voir dans une sténose aortique du fait d’une contrainte sigma du ventricule  gauche augmentée même si la tension artérielle est basse.   </t>
+  </si>
+  <si>
+    <t>Si la fraction d'ejection est de 30%, elle est en dessous de 40% (cptn obvious) et donc si la contrainte sigma a augmenté, ça veut dire que la postcharge a augmenté donc on est dans le cas en haut à droite sur l'image. Or la tension artérielle reste basse, donc on est obligatoirement en sténose aortique</t>
+  </si>
+  <si>
+    <t>Si il y a une hypertension artérielle systémique, ça veut dire que l'axe électrique du cœur aura tendance à s'orienter vers la gauche (pour bien bien innerver le ventricule gauche) et donc le complexe QRS (qui représente l'axe electrique du cœur) peut apparaitre nul en DII (isoelectrique quoi) et negatif en aVF</t>
+  </si>
+  <si>
+    <t>epicarde vers endocarde</t>
+  </si>
+  <si>
+    <t>la resistance cardiaque diminue moins que le debit cardiaque augmente</t>
+  </si>
+  <si>
+    <t>ça affecte la fonction diastolique (la compliance reflete l'elastance vu que c'est l'inverse l'un de l'autre)</t>
+  </si>
+  <si>
+    <t>A cause de l'hypertrophie, le muscle du ventricule gauche sera bcp plus epais, donc le remplissage du ventricule gauche sera diminué -&gt; précharge diminue. De même, parceque le muscle sera plus epais, il sera plus tendu -&gt; diminution de la postcharge</t>
+  </si>
+  <si>
+    <t>Le retour veineux va influer sur le volume telediastolique, mais n'aura donc aucun rapport avec le volume telesystolique. Il n'y aura donc aucun changement de la droite d'elastance en fin de systole</t>
+  </si>
+  <si>
+    <t>L'erreur ici c'est que chronotrope = frequence cardiaque et dromotrope = vitesse de conduction</t>
   </si>
 </sst>
 </file>
@@ -1664,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4434D7D-6CBE-4AEC-87F6-B0BB4C058CB9}">
-  <dimension ref="A1:F260"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -1771,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -1785,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1811,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -1831,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1891,7 +1876,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1925,7 +1910,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1971,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1991,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -2011,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -2071,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -2151,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -2171,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -2191,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -2291,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -2331,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -2365,13 +2350,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -2451,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -2511,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -2551,7 +2536,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -2631,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -2651,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -2691,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -2705,13 +2690,13 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -2785,13 +2770,13 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -2871,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="F60" t="s">
         <v>6</v>
@@ -2911,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="F62" t="s">
         <v>6</v>
@@ -2971,7 +2956,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="F65" t="s">
         <v>6</v>
@@ -2991,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="F66" t="s">
         <v>6</v>
@@ -3025,7 +3010,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -3151,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="F74" t="s">
         <v>6</v>
@@ -3171,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="F75" t="s">
         <v>6</v>
@@ -3191,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
@@ -3205,7 +3190,7 @@
         <v>81</v>
       </c>
       <c r="C77" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -3231,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
@@ -3251,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -3271,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
@@ -3285,7 +3270,7 @@
         <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -3305,13 +3290,13 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -3331,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -3351,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -3371,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -3379,13 +3364,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>90</v>
       </c>
       <c r="C86" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -3399,7 +3384,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>90</v>
@@ -3419,19 +3404,19 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>
@@ -3439,7 +3424,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>92</v>
@@ -3459,7 +3444,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>92</v>
@@ -3479,7 +3464,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>92</v>
@@ -3491,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="F91" t="s">
         <v>6</v>
@@ -3499,7 +3484,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>96</v>
@@ -3519,7 +3504,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>96</v>
@@ -3539,7 +3524,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>96</v>
@@ -3551,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F94" t="s">
         <v>6</v>
@@ -3559,7 +3544,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>100</v>
@@ -3579,7 +3564,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>100</v>
@@ -3599,7 +3584,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>100</v>
@@ -3619,7 +3604,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>104</v>
@@ -3631,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F98" t="s">
         <v>6</v>
@@ -3639,7 +3624,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>104</v>
@@ -3659,13 +3644,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>104</v>
       </c>
       <c r="C100" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -3679,7 +3664,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -3691,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
@@ -3699,7 +3684,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -3711,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="F102" t="s">
         <v>6</v>
@@ -3719,19 +3704,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="F103" t="s">
         <v>6</v>
@@ -3739,7 +3724,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>109</v>
@@ -3751,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="F104" t="s">
         <v>6</v>
@@ -3759,7 +3744,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>109</v>
@@ -3779,7 +3764,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>109</v>
@@ -3799,7 +3784,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>113</v>
@@ -3819,7 +3804,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>113</v>
@@ -3831,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="F108" t="s">
         <v>6</v>
@@ -3839,13 +3824,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>113</v>
       </c>
       <c r="C109" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -3859,13 +3844,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>116</v>
       </c>
       <c r="C110" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -3879,7 +3864,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>116</v>
@@ -3891,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="E111" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="F111" t="s">
         <v>6</v>
@@ -3899,7 +3884,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
         <v>118</v>
@@ -3919,7 +3904,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>118</v>
@@ -3939,13 +3924,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>121</v>
       </c>
       <c r="C114" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -3959,7 +3944,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>121</v>
@@ -3979,7 +3964,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>121</v>
@@ -3991,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="F116" t="s">
         <v>6</v>
@@ -3999,19 +3984,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>124</v>
       </c>
       <c r="C117" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="D117" t="b">
         <v>0</v>
       </c>
       <c r="E117" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="F117" t="s">
         <v>6</v>
@@ -4019,7 +4004,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>124</v>
@@ -4039,7 +4024,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>124</v>
@@ -4059,7 +4044,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -4079,7 +4064,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
@@ -4099,7 +4084,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -4119,7 +4104,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -4139,7 +4124,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
@@ -4159,7 +4144,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -4171,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="F125" t="s">
         <v>6</v>
@@ -4179,7 +4164,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -4191,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="F126" t="s">
         <v>6</v>
@@ -4199,7 +4184,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
@@ -4219,7 +4204,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -4231,7 +4216,7 @@
         <v>0</v>
       </c>
       <c r="E128" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="F128" t="s">
         <v>6</v>
@@ -4239,7 +4224,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -4251,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="F129" t="s">
         <v>6</v>
@@ -4259,13 +4244,13 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="D130" t="b">
         <v>1</v>
@@ -4279,7 +4264,7 @@
     </row>
     <row r="131" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -4299,7 +4284,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -4319,7 +4304,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s">
         <v>6</v>
@@ -4339,7 +4324,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B134" t="s">
         <v>6</v>
@@ -4359,7 +4344,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
         <v>6</v>
@@ -4371,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="E135" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F135" t="s">
         <v>6</v>
@@ -4379,7 +4364,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -4399,7 +4384,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
         <v>6</v>
@@ -4411,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="E137" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="F137" t="s">
         <v>6</v>
@@ -4419,7 +4404,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
         <v>144</v>
@@ -4431,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="E138" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="F138" t="s">
         <v>6</v>
@@ -4439,7 +4424,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
         <v>144</v>
@@ -4451,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="E139" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="F139" t="s">
         <v>6</v>
@@ -4459,7 +4444,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -4471,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="E140" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="F140" t="s">
         <v>6</v>
@@ -4479,7 +4464,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
         <v>148</v>
@@ -4499,13 +4484,13 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s">
         <v>148</v>
       </c>
       <c r="C142" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="D142" t="b">
         <v>1</v>
@@ -4519,7 +4504,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
         <v>148</v>
@@ -4531,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="E143" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="F143" t="s">
         <v>6</v>
@@ -4539,7 +4524,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
         <v>151</v>
@@ -4559,7 +4544,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B145" t="s">
         <v>151</v>
@@ -4571,7 +4556,7 @@
         <v>0</v>
       </c>
       <c r="E145" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="F145" t="s">
         <v>6</v>
@@ -4579,7 +4564,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B146" t="s">
         <v>151</v>
@@ -4599,19 +4584,19 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B147" t="s">
         <v>155</v>
       </c>
       <c r="C147" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="D147" t="b">
         <v>0</v>
       </c>
       <c r="E147" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="F147" t="s">
         <v>6</v>
@@ -4619,19 +4604,19 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B148" t="s">
         <v>155</v>
       </c>
       <c r="C148" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="D148" t="b">
         <v>0</v>
       </c>
       <c r="E148" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="F148" t="s">
         <v>6</v>
@@ -4639,7 +4624,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B149" t="s">
         <v>155</v>
@@ -4659,7 +4644,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B150" t="s">
         <v>157</v>
@@ -4671,7 +4656,7 @@
         <v>1</v>
       </c>
       <c r="E150" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="F150" t="s">
         <v>6</v>
@@ -4679,7 +4664,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B151" t="s">
         <v>157</v>
@@ -4699,7 +4684,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
         <v>157</v>
@@ -4719,7 +4704,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>161</v>
@@ -4739,13 +4724,13 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>161</v>
       </c>
       <c r="C154" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="D154" t="b">
         <v>1</v>
@@ -4759,7 +4744,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>161</v>
@@ -4771,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="E155" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="F155" t="s">
         <v>6</v>
@@ -4779,7 +4764,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B156" t="s">
         <v>164</v>
@@ -4799,7 +4784,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B157" t="s">
         <v>164</v>
@@ -4819,7 +4804,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B158" t="s">
         <v>164</v>
@@ -4831,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="E158" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="F158" t="s">
         <v>6</v>
@@ -4839,7 +4824,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B159" t="s">
         <v>168</v>
@@ -4851,7 +4836,7 @@
         <v>1</v>
       </c>
       <c r="E159" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="F159" t="s">
         <v>6</v>
@@ -4859,7 +4844,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>170</v>
@@ -4879,7 +4864,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B161" t="s">
         <v>170</v>
@@ -4891,7 +4876,7 @@
         <v>0</v>
       </c>
       <c r="E161" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="F161" t="s">
         <v>6</v>
@@ -4899,7 +4884,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B162" t="s">
         <v>170</v>
@@ -4911,7 +4896,7 @@
         <v>1</v>
       </c>
       <c r="E162" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="F162" t="s">
         <v>6</v>
@@ -4919,7 +4904,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B163" t="s">
         <v>174</v>
@@ -4931,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="E163" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="F163" t="s">
         <v>6</v>
@@ -4939,7 +4924,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>174</v>
@@ -4959,7 +4944,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B165" t="s">
         <v>174</v>
@@ -4971,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="E165" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="F165" t="s">
         <v>6</v>
@@ -4979,7 +4964,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B166" t="s">
         <v>178</v>
@@ -4999,7 +4984,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B167" t="s">
         <v>178</v>
@@ -5019,7 +5004,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B168" t="s">
         <v>178</v>
@@ -5031,7 +5016,7 @@
         <v>0</v>
       </c>
       <c r="E168" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="F168" t="s">
         <v>6</v>
@@ -5039,13 +5024,13 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B169" t="s">
         <v>182</v>
       </c>
       <c r="C169" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="D169" t="b">
         <v>1</v>
@@ -5059,7 +5044,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B170" t="s">
         <v>182</v>
@@ -5079,7 +5064,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B171" t="s">
         <v>184</v>
@@ -5099,7 +5084,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B172" t="s">
         <v>184</v>
@@ -5111,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="E172" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F172" t="s">
         <v>6</v>
@@ -5119,7 +5104,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B173" t="s">
         <v>184</v>
@@ -5131,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="E173" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="F173" t="s">
         <v>6</v>
@@ -5139,7 +5124,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B174" t="s">
         <v>188</v>
@@ -5159,7 +5144,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B175" t="s">
         <v>188</v>
@@ -5171,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="E175" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="F175" t="s">
         <v>6</v>
@@ -5179,7 +5164,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B176" t="s">
         <v>188</v>
@@ -5199,7 +5184,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B177" t="s">
         <v>192</v>
@@ -5219,7 +5204,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B178" t="s">
         <v>192</v>
@@ -5239,7 +5224,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B179" t="s">
         <v>192</v>
@@ -5251,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="E179" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="F179" t="s">
         <v>6</v>
@@ -5259,7 +5244,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B180" t="s">
         <v>196</v>
@@ -5279,7 +5264,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
         <v>196</v>
@@ -5291,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="E181" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="F181" t="s">
         <v>6</v>
@@ -5299,7 +5284,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B182" t="s">
         <v>196</v>
@@ -5319,7 +5304,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B183" t="s">
         <v>200</v>
@@ -5339,7 +5324,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B184" t="s">
         <v>202</v>
@@ -5351,7 +5336,7 @@
         <v>0</v>
       </c>
       <c r="E184" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="F184" t="s">
         <v>6</v>
@@ -5359,7 +5344,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B185" t="s">
         <v>202</v>
@@ -5379,7 +5364,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B186" t="s">
         <v>202</v>
@@ -5399,7 +5384,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B187" t="s">
         <v>206</v>
@@ -5419,7 +5404,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B188" t="s">
         <v>206</v>
@@ -5439,7 +5424,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B189" t="s">
         <v>206</v>
@@ -5459,13 +5444,13 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B190" t="s">
         <v>210</v>
       </c>
       <c r="C190" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="D190" t="b">
         <v>1</v>
@@ -5479,7 +5464,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B191" t="s">
         <v>210</v>
@@ -5491,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="E191" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="F191" t="s">
         <v>6</v>
@@ -5499,7 +5484,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B192" t="s">
         <v>210</v>
@@ -5519,7 +5504,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B193" t="s">
         <v>213</v>
@@ -5531,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="E193" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="F193" t="s">
         <v>6</v>
@@ -5539,19 +5524,19 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B194" t="s">
         <v>213</v>
       </c>
       <c r="C194" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="D194" t="b">
         <v>1</v>
       </c>
       <c r="E194" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="F194" t="s">
         <v>6</v>
@@ -5559,7 +5544,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B195" t="s">
         <v>213</v>
@@ -5579,7 +5564,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B196" t="s">
         <v>216</v>
@@ -5591,7 +5576,7 @@
         <v>0</v>
       </c>
       <c r="E196" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="F196" t="s">
         <v>6</v>
@@ -5599,7 +5584,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B197" t="s">
         <v>218</v>
@@ -5619,7 +5604,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B198" t="s">
         <v>218</v>
@@ -5639,13 +5624,13 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C199" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="D199" t="b">
         <v>0</v>
@@ -5659,10 +5644,10 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C200" t="s">
         <v>221</v>
@@ -5671,7 +5656,7 @@
         <v>0</v>
       </c>
       <c r="E200" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="F200" t="s">
         <v>6</v>
@@ -5679,10 +5664,10 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C201" t="s">
         <v>222</v>
@@ -5691,7 +5676,7 @@
         <v>0</v>
       </c>
       <c r="E201" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="F201" t="s">
         <v>6</v>
@@ -5699,7 +5684,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B202" t="s">
         <v>223</v>
@@ -5719,7 +5704,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B203" t="s">
         <v>223</v>
@@ -5739,13 +5724,13 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B204" t="s">
         <v>223</v>
       </c>
       <c r="C204" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="D204" t="b">
         <v>0</v>
@@ -5759,7 +5744,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="B205" t="s">
         <v>226</v>
@@ -5779,7 +5764,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="B206" t="s">
         <v>226</v>
@@ -5799,7 +5784,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B207" t="s">
         <v>229</v>
@@ -5819,7 +5804,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="B208" t="s">
         <v>229</v>
@@ -5839,19 +5824,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C209" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D209" t="b">
         <v>1</v>
       </c>
       <c r="E209" t="s">
-        <v>6</v>
+        <v>388</v>
       </c>
       <c r="F209" t="s">
         <v>6</v>
@@ -5859,13 +5844,13 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C210" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D210" t="b">
         <v>0</v>
@@ -5879,13 +5864,13 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C211" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D211" t="b">
         <v>1</v>
@@ -5899,19 +5884,19 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C212" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D212" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E212" t="s">
-        <v>6</v>
+        <v>309</v>
       </c>
       <c r="F212" t="s">
         <v>6</v>
@@ -5919,16 +5904,16 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B213" t="s">
         <v>237</v>
       </c>
       <c r="C213" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E213" t="s">
         <v>6</v>
@@ -5939,16 +5924,16 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C214" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D214" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E214" t="s">
         <v>6</v>
@@ -5959,13 +5944,13 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C215" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D215" t="b">
         <v>1</v>
@@ -5979,19 +5964,19 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C216" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D216" t="b">
         <v>0</v>
       </c>
       <c r="E216" t="s">
-        <v>6</v>
+        <v>389</v>
       </c>
       <c r="F216" t="s">
         <v>6</v>
@@ -5999,19 +5984,19 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C217" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D217" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E217" t="s">
-        <v>6</v>
+        <v>390</v>
       </c>
       <c r="F217" t="s">
         <v>6</v>
@@ -6019,13 +6004,13 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C218" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D218" t="b">
         <v>1</v>
@@ -6039,13 +6024,13 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C219" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D219" t="b">
         <v>1</v>
@@ -6059,13 +6044,13 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C220" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D220" t="b">
         <v>1</v>
@@ -6079,16 +6064,16 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C221" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D221" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E221" t="s">
         <v>6</v>
@@ -6099,19 +6084,19 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C222" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D222" t="b">
         <v>0</v>
       </c>
       <c r="E222" t="s">
-        <v>6</v>
+        <v>391</v>
       </c>
       <c r="F222" t="s">
         <v>6</v>
@@ -6119,19 +6104,19 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C223" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D223" t="b">
         <v>1</v>
       </c>
       <c r="E223" t="s">
-        <v>6</v>
+        <v>392</v>
       </c>
       <c r="F223" t="s">
         <v>6</v>
@@ -6139,19 +6124,19 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C224" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D224" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E224" t="s">
-        <v>6</v>
+        <v>393</v>
       </c>
       <c r="F224" t="s">
         <v>6</v>
@@ -6159,16 +6144,16 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="C225" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D225" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E225" t="s">
         <v>6</v>
@@ -6179,19 +6164,19 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="C226" t="s">
-        <v>254</v>
+        <v>394</v>
       </c>
       <c r="D226" t="b">
         <v>1</v>
       </c>
       <c r="E226" t="s">
-        <v>6</v>
+        <v>395</v>
       </c>
       <c r="F226" t="s">
         <v>6</v>
@@ -6199,13 +6184,13 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="C227" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D227" t="b">
         <v>1</v>
@@ -6219,19 +6204,19 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C228" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D228" t="b">
         <v>1</v>
       </c>
       <c r="E228" t="s">
-        <v>6</v>
+        <v>396</v>
       </c>
       <c r="F228" t="s">
         <v>6</v>
@@ -6239,13 +6224,13 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C229" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D229" t="b">
         <v>1</v>
@@ -6259,13 +6244,13 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C230" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D230" t="b">
         <v>1</v>
@@ -6279,13 +6264,13 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C231" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D231" t="b">
         <v>0</v>
@@ -6299,13 +6284,13 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C232" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D232" t="b">
         <v>1</v>
@@ -6319,19 +6304,19 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C233" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D233" t="b">
         <v>0</v>
       </c>
       <c r="E233" t="s">
-        <v>6</v>
+        <v>397</v>
       </c>
       <c r="F233" t="s">
         <v>6</v>
@@ -6339,19 +6324,19 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C234" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D234" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E234" t="s">
-        <v>6</v>
+        <v>398</v>
       </c>
       <c r="F234" t="s">
         <v>6</v>
@@ -6359,13 +6344,13 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C235" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D235" t="b">
         <v>1</v>
@@ -6379,13 +6364,13 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C236" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D236" t="b">
         <v>1</v>
@@ -6399,19 +6384,19 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C237" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D237" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E237" t="s">
-        <v>6</v>
+        <v>399</v>
       </c>
       <c r="F237" t="s">
         <v>6</v>
@@ -6419,19 +6404,19 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C238" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D238" t="b">
         <v>1</v>
       </c>
       <c r="E238" t="s">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="F238" t="s">
         <v>6</v>
@@ -6439,19 +6424,19 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C239" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D239" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E239" t="s">
-        <v>6</v>
+        <v>401</v>
       </c>
       <c r="F239" t="s">
         <v>6</v>
@@ -6459,19 +6444,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C240" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D240" t="b">
         <v>0</v>
       </c>
       <c r="E240" t="s">
-        <v>6</v>
+        <v>402</v>
       </c>
       <c r="F240" t="s">
         <v>6</v>
@@ -6479,13 +6464,13 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C241" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D241" t="b">
         <v>1</v>
@@ -6499,16 +6484,16 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C242" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D242" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E242" t="s">
         <v>6</v>
@@ -6519,13 +6504,13 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C243" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D243" t="b">
         <v>0</v>
@@ -6534,346 +6519,6 @@
         <v>6</v>
       </c>
       <c r="F243" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
-        <v>260</v>
-      </c>
-      <c r="B244" t="s">
-        <v>276</v>
-      </c>
-      <c r="C244" t="s">
-        <v>278</v>
-      </c>
-      <c r="D244" t="b">
-        <v>1</v>
-      </c>
-      <c r="E244" t="s">
-        <v>6</v>
-      </c>
-      <c r="F244" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
-        <v>261</v>
-      </c>
-      <c r="B245" t="s">
-        <v>276</v>
-      </c>
-      <c r="C245" t="s">
-        <v>279</v>
-      </c>
-      <c r="D245" t="b">
-        <v>1</v>
-      </c>
-      <c r="E245" t="s">
-        <v>6</v>
-      </c>
-      <c r="F245" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
-        <v>262</v>
-      </c>
-      <c r="B246" t="s">
-        <v>280</v>
-      </c>
-      <c r="C246" t="s">
-        <v>281</v>
-      </c>
-      <c r="D246" t="b">
-        <v>0</v>
-      </c>
-      <c r="E246" t="s">
-        <v>6</v>
-      </c>
-      <c r="F246" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
-        <v>263</v>
-      </c>
-      <c r="B247" t="s">
-        <v>280</v>
-      </c>
-      <c r="C247" t="s">
-        <v>282</v>
-      </c>
-      <c r="D247" t="b">
-        <v>1</v>
-      </c>
-      <c r="E247" t="s">
-        <v>6</v>
-      </c>
-      <c r="F247" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" s="1">
-        <v>264</v>
-      </c>
-      <c r="B248" t="s">
-        <v>280</v>
-      </c>
-      <c r="C248" t="s">
-        <v>283</v>
-      </c>
-      <c r="D248" t="b">
-        <v>0</v>
-      </c>
-      <c r="E248" t="s">
-        <v>6</v>
-      </c>
-      <c r="F248" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="1">
-        <v>265</v>
-      </c>
-      <c r="B249" t="s">
-        <v>284</v>
-      </c>
-      <c r="C249" t="s">
-        <v>285</v>
-      </c>
-      <c r="D249" t="b">
-        <v>0</v>
-      </c>
-      <c r="E249" t="s">
-        <v>6</v>
-      </c>
-      <c r="F249" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
-        <v>266</v>
-      </c>
-      <c r="B250" t="s">
-        <v>284</v>
-      </c>
-      <c r="C250" t="s">
-        <v>286</v>
-      </c>
-      <c r="D250" t="b">
-        <v>0</v>
-      </c>
-      <c r="E250" t="s">
-        <v>6</v>
-      </c>
-      <c r="F250" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="1">
-        <v>267</v>
-      </c>
-      <c r="B251" t="s">
-        <v>284</v>
-      </c>
-      <c r="C251" t="s">
-        <v>287</v>
-      </c>
-      <c r="D251" t="b">
-        <v>1</v>
-      </c>
-      <c r="E251" t="s">
-        <v>6</v>
-      </c>
-      <c r="F251" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
-        <v>268</v>
-      </c>
-      <c r="B252" t="s">
-        <v>288</v>
-      </c>
-      <c r="C252" t="s">
-        <v>289</v>
-      </c>
-      <c r="D252" t="b">
-        <v>1</v>
-      </c>
-      <c r="E252" t="s">
-        <v>6</v>
-      </c>
-      <c r="F252" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A253" s="1">
-        <v>269</v>
-      </c>
-      <c r="B253" t="s">
-        <v>288</v>
-      </c>
-      <c r="C253" t="s">
-        <v>290</v>
-      </c>
-      <c r="D253" t="b">
-        <v>0</v>
-      </c>
-      <c r="E253" t="s">
-        <v>6</v>
-      </c>
-      <c r="F253" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A254" s="1">
-        <v>270</v>
-      </c>
-      <c r="B254" t="s">
-        <v>288</v>
-      </c>
-      <c r="C254" t="s">
-        <v>291</v>
-      </c>
-      <c r="D254" t="b">
-        <v>0</v>
-      </c>
-      <c r="E254" t="s">
-        <v>6</v>
-      </c>
-      <c r="F254" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
-        <v>271</v>
-      </c>
-      <c r="B255" t="s">
-        <v>292</v>
-      </c>
-      <c r="C255" t="s">
-        <v>293</v>
-      </c>
-      <c r="D255" t="b">
-        <v>1</v>
-      </c>
-      <c r="E255" t="s">
-        <v>6</v>
-      </c>
-      <c r="F255" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" s="1">
-        <v>272</v>
-      </c>
-      <c r="B256" t="s">
-        <v>292</v>
-      </c>
-      <c r="C256" t="s">
-        <v>294</v>
-      </c>
-      <c r="D256" t="b">
-        <v>0</v>
-      </c>
-      <c r="E256" t="s">
-        <v>6</v>
-      </c>
-      <c r="F256" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A257" s="1">
-        <v>273</v>
-      </c>
-      <c r="B257" t="s">
-        <v>292</v>
-      </c>
-      <c r="C257" t="s">
-        <v>295</v>
-      </c>
-      <c r="D257" t="b">
-        <v>1</v>
-      </c>
-      <c r="E257" t="s">
-        <v>6</v>
-      </c>
-      <c r="F257" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A258" s="1">
-        <v>274</v>
-      </c>
-      <c r="B258" t="s">
-        <v>296</v>
-      </c>
-      <c r="C258" t="s">
-        <v>297</v>
-      </c>
-      <c r="D258" t="b">
-        <v>1</v>
-      </c>
-      <c r="E258" t="s">
-        <v>6</v>
-      </c>
-      <c r="F258" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A259" s="1">
-        <v>275</v>
-      </c>
-      <c r="B259" t="s">
-        <v>296</v>
-      </c>
-      <c r="C259" t="s">
-        <v>298</v>
-      </c>
-      <c r="D259" t="b">
-        <v>1</v>
-      </c>
-      <c r="E259" t="s">
-        <v>6</v>
-      </c>
-      <c r="F259" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" s="1">
-        <v>276</v>
-      </c>
-      <c r="B260" t="s">
-        <v>296</v>
-      </c>
-      <c r="C260" t="s">
-        <v>299</v>
-      </c>
-      <c r="D260" t="b">
-        <v>0</v>
-      </c>
-      <c r="E260" t="s">
-        <v>6</v>
-      </c>
-      <c r="F260" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>